<commit_message>
Adding comments to Example2...
</commit_message>
<xml_diff>
--- a/Examples/Trello.xlsx
+++ b/Examples/Trello.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\detle\Documents\GitHub\Get-Trello\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BBCFA3-CC03-4D16-8B49-C2C72E77494D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFD11D7-A0A2-47F5-B585-39C53AB3EA30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="0" windowWidth="27855" windowHeight="12750" xr2:uid="{C600EE37-929E-4CD4-88D7-44DCAC1720A4}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="27855" windowHeight="12750" xr2:uid="{C600EE37-929E-4CD4-88D7-44DCAC1720A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trello Tasks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>